<commit_message>
added info for dry ice
</commit_message>
<xml_diff>
--- a/cites_list.xlsx
+++ b/cites_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD63BED7-B337-9349-95BD-1912E50879CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D535A09-259C-DB4D-92D4-A2745A2B85F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="760" windowWidth="21180" windowHeight="17060" xr2:uid="{3910AC6C-398B-5641-A261-4AC5E77A0DDB}"/>
+    <workbookView xWindow="-29020" yWindow="-380" windowWidth="21180" windowHeight="17060" xr2:uid="{3910AC6C-398B-5641-A261-4AC5E77A0DDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3814" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3814" uniqueCount="356">
   <si>
     <t>species</t>
   </si>
@@ -1101,6 +1101,9 @@
   </si>
   <si>
     <t>TOTAL SAMPLES</t>
+  </si>
+  <si>
+    <t>Dry shipper or dry ice</t>
   </si>
 </sst>
 </file>
@@ -1196,9 +1199,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1236,7 +1239,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1342,7 +1345,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1484,7 +1487,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1494,9 +1497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B8E095-94BA-A842-9ABD-01710D83669F}">
   <dimension ref="A1:M577"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A472" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I288" sqref="I288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5128,7 +5131,7 @@
         <v>148</v>
       </c>
       <c r="G153" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
@@ -5151,7 +5154,7 @@
         <v>148</v>
       </c>
       <c r="G154" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
@@ -5174,7 +5177,7 @@
         <v>148</v>
       </c>
       <c r="G155" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
@@ -5197,7 +5200,7 @@
         <v>148</v>
       </c>
       <c r="G156" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
@@ -5220,7 +5223,7 @@
         <v>148</v>
       </c>
       <c r="G157" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
@@ -5243,7 +5246,7 @@
         <v>148</v>
       </c>
       <c r="G158" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
@@ -5266,7 +5269,7 @@
         <v>148</v>
       </c>
       <c r="G159" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
@@ -5289,7 +5292,7 @@
         <v>148</v>
       </c>
       <c r="G160" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
@@ -5312,7 +5315,7 @@
         <v>148</v>
       </c>
       <c r="G161" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
@@ -5335,7 +5338,7 @@
         <v>148</v>
       </c>
       <c r="G162" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
@@ -5358,7 +5361,7 @@
         <v>148</v>
       </c>
       <c r="G163" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
@@ -5381,7 +5384,7 @@
         <v>148</v>
       </c>
       <c r="G164" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
@@ -5404,7 +5407,7 @@
         <v>148</v>
       </c>
       <c r="G165" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
@@ -5427,7 +5430,7 @@
         <v>148</v>
       </c>
       <c r="G166" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
@@ -5450,7 +5453,7 @@
         <v>148</v>
       </c>
       <c r="G167" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
@@ -5473,7 +5476,7 @@
         <v>148</v>
       </c>
       <c r="G168" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
@@ -5496,7 +5499,7 @@
         <v>148</v>
       </c>
       <c r="G169" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
@@ -5519,7 +5522,7 @@
         <v>148</v>
       </c>
       <c r="G170" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
@@ -5542,7 +5545,7 @@
         <v>148</v>
       </c>
       <c r="G171" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
@@ -5565,7 +5568,7 @@
         <v>148</v>
       </c>
       <c r="G172" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
@@ -5588,7 +5591,7 @@
         <v>148</v>
       </c>
       <c r="G173" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
@@ -5611,7 +5614,7 @@
         <v>148</v>
       </c>
       <c r="G174" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
@@ -5634,7 +5637,7 @@
         <v>148</v>
       </c>
       <c r="G175" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
@@ -5657,7 +5660,7 @@
         <v>148</v>
       </c>
       <c r="G176" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
@@ -5680,7 +5683,7 @@
         <v>148</v>
       </c>
       <c r="G177" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
@@ -5703,7 +5706,7 @@
         <v>148</v>
       </c>
       <c r="G178" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
@@ -5726,7 +5729,7 @@
         <v>148</v>
       </c>
       <c r="G179" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.2">
@@ -5749,7 +5752,7 @@
         <v>148</v>
       </c>
       <c r="G180" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
@@ -5772,7 +5775,7 @@
         <v>148</v>
       </c>
       <c r="G181" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
@@ -5795,7 +5798,7 @@
         <v>148</v>
       </c>
       <c r="G182" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.2">
@@ -5818,7 +5821,7 @@
         <v>148</v>
       </c>
       <c r="G183" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
@@ -5841,7 +5844,7 @@
         <v>148</v>
       </c>
       <c r="G184" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
@@ -5864,7 +5867,7 @@
         <v>148</v>
       </c>
       <c r="G185" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
@@ -5887,7 +5890,7 @@
         <v>148</v>
       </c>
       <c r="G186" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
@@ -5910,7 +5913,7 @@
         <v>148</v>
       </c>
       <c r="G187" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.2">
@@ -5933,7 +5936,7 @@
         <v>148</v>
       </c>
       <c r="G188" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
@@ -5956,7 +5959,7 @@
         <v>148</v>
       </c>
       <c r="G189" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
@@ -5979,7 +5982,7 @@
         <v>148</v>
       </c>
       <c r="G190" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
@@ -6002,7 +6005,7 @@
         <v>148</v>
       </c>
       <c r="G191" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.2">
@@ -6025,7 +6028,7 @@
         <v>148</v>
       </c>
       <c r="G192" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.2">
@@ -6048,7 +6051,7 @@
         <v>148</v>
       </c>
       <c r="G193" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.2">
@@ -6071,7 +6074,7 @@
         <v>148</v>
       </c>
       <c r="G194" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.2">
@@ -6094,7 +6097,7 @@
         <v>148</v>
       </c>
       <c r="G195" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.2">
@@ -6117,7 +6120,7 @@
         <v>148</v>
       </c>
       <c r="G196" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.2">
@@ -6140,7 +6143,7 @@
         <v>148</v>
       </c>
       <c r="G197" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.2">
@@ -6163,7 +6166,7 @@
         <v>148</v>
       </c>
       <c r="G198" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.2">
@@ -6186,7 +6189,7 @@
         <v>148</v>
       </c>
       <c r="G199" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.2">
@@ -6209,7 +6212,7 @@
         <v>148</v>
       </c>
       <c r="G200" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.2">
@@ -6232,7 +6235,7 @@
         <v>148</v>
       </c>
       <c r="G201" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.2">
@@ -6255,7 +6258,7 @@
         <v>148</v>
       </c>
       <c r="G202" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.2">
@@ -6278,7 +6281,7 @@
         <v>148</v>
       </c>
       <c r="G203" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.2">
@@ -6301,7 +6304,7 @@
         <v>148</v>
       </c>
       <c r="G204" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.2">
@@ -6324,7 +6327,7 @@
         <v>148</v>
       </c>
       <c r="G205" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.2">
@@ -6347,7 +6350,7 @@
         <v>148</v>
       </c>
       <c r="G206" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.2">
@@ -6370,7 +6373,7 @@
         <v>148</v>
       </c>
       <c r="G207" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.2">
@@ -6393,7 +6396,7 @@
         <v>148</v>
       </c>
       <c r="G208" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.2">
@@ -6416,7 +6419,7 @@
         <v>148</v>
       </c>
       <c r="G209" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.2">
@@ -6439,7 +6442,7 @@
         <v>148</v>
       </c>
       <c r="G210" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.2">
@@ -6462,7 +6465,7 @@
         <v>148</v>
       </c>
       <c r="G211" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.2">
@@ -6485,7 +6488,7 @@
         <v>148</v>
       </c>
       <c r="G212" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.2">
@@ -6508,7 +6511,7 @@
         <v>148</v>
       </c>
       <c r="G213" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.2">
@@ -6531,7 +6534,7 @@
         <v>148</v>
       </c>
       <c r="G214" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.2">
@@ -6554,7 +6557,7 @@
         <v>148</v>
       </c>
       <c r="G215" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.2">
@@ -6577,7 +6580,7 @@
         <v>148</v>
       </c>
       <c r="G216" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.2">
@@ -6600,7 +6603,7 @@
         <v>148</v>
       </c>
       <c r="G217" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.2">
@@ -6623,7 +6626,7 @@
         <v>148</v>
       </c>
       <c r="G218" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.2">
@@ -6646,7 +6649,7 @@
         <v>148</v>
       </c>
       <c r="G219" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.2">
@@ -6669,7 +6672,7 @@
         <v>148</v>
       </c>
       <c r="G220" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.2">
@@ -6692,7 +6695,7 @@
         <v>148</v>
       </c>
       <c r="G221" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.2">
@@ -6715,7 +6718,7 @@
         <v>148</v>
       </c>
       <c r="G222" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.2">
@@ -6738,7 +6741,7 @@
         <v>148</v>
       </c>
       <c r="G223" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.2">
@@ -6761,7 +6764,7 @@
         <v>148</v>
       </c>
       <c r="G224" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.2">
@@ -6784,7 +6787,7 @@
         <v>148</v>
       </c>
       <c r="G225" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.2">
@@ -6807,7 +6810,7 @@
         <v>148</v>
       </c>
       <c r="G226" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.2">
@@ -6830,7 +6833,7 @@
         <v>148</v>
       </c>
       <c r="G227" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.2">
@@ -6853,7 +6856,7 @@
         <v>148</v>
       </c>
       <c r="G228" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.2">
@@ -6876,7 +6879,7 @@
         <v>148</v>
       </c>
       <c r="G229" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.2">
@@ -6899,7 +6902,7 @@
         <v>148</v>
       </c>
       <c r="G230" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.2">
@@ -6922,7 +6925,7 @@
         <v>148</v>
       </c>
       <c r="G231" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.2">
@@ -6945,7 +6948,7 @@
         <v>148</v>
       </c>
       <c r="G232" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.2">
@@ -6968,7 +6971,7 @@
         <v>148</v>
       </c>
       <c r="G233" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.2">
@@ -6991,7 +6994,7 @@
         <v>148</v>
       </c>
       <c r="G234" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.2">
@@ -7014,7 +7017,7 @@
         <v>148</v>
       </c>
       <c r="G235" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.2">
@@ -7037,7 +7040,7 @@
         <v>148</v>
       </c>
       <c r="G236" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.2">
@@ -7060,7 +7063,7 @@
         <v>148</v>
       </c>
       <c r="G237" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.2">
@@ -7083,7 +7086,7 @@
         <v>148</v>
       </c>
       <c r="G238" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.2">
@@ -7106,7 +7109,7 @@
         <v>148</v>
       </c>
       <c r="G239" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.2">
@@ -7129,7 +7132,7 @@
         <v>148</v>
       </c>
       <c r="G240" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.2">
@@ -7152,7 +7155,7 @@
         <v>148</v>
       </c>
       <c r="G241" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.2">
@@ -7175,7 +7178,7 @@
         <v>148</v>
       </c>
       <c r="G242" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.2">
@@ -7198,7 +7201,7 @@
         <v>148</v>
       </c>
       <c r="G243" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.2">
@@ -7221,7 +7224,7 @@
         <v>148</v>
       </c>
       <c r="G244" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.2">
@@ -7244,7 +7247,7 @@
         <v>148</v>
       </c>
       <c r="G245" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.2">
@@ -7267,7 +7270,7 @@
         <v>148</v>
       </c>
       <c r="G246" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.2">
@@ -7290,7 +7293,7 @@
         <v>148</v>
       </c>
       <c r="G247" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.2">
@@ -7313,7 +7316,7 @@
         <v>148</v>
       </c>
       <c r="G248" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.2">
@@ -7336,7 +7339,7 @@
         <v>148</v>
       </c>
       <c r="G249" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.2">
@@ -7359,7 +7362,7 @@
         <v>148</v>
       </c>
       <c r="G250" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.2">
@@ -7382,7 +7385,7 @@
         <v>148</v>
       </c>
       <c r="G251" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.2">
@@ -7405,7 +7408,7 @@
         <v>148</v>
       </c>
       <c r="G252" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.2">
@@ -7428,7 +7431,7 @@
         <v>148</v>
       </c>
       <c r="G253" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.2">
@@ -7451,7 +7454,7 @@
         <v>148</v>
       </c>
       <c r="G254" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.2">
@@ -7474,7 +7477,7 @@
         <v>148</v>
       </c>
       <c r="G255" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.2">
@@ -7497,7 +7500,7 @@
         <v>148</v>
       </c>
       <c r="G256" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.2">
@@ -7520,7 +7523,7 @@
         <v>148</v>
       </c>
       <c r="G257" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.2">
@@ -7543,7 +7546,7 @@
         <v>148</v>
       </c>
       <c r="G258" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.2">
@@ -7566,7 +7569,7 @@
         <v>148</v>
       </c>
       <c r="G259" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.2">
@@ -7589,7 +7592,7 @@
         <v>148</v>
       </c>
       <c r="G260" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.2">
@@ -7612,7 +7615,7 @@
         <v>148</v>
       </c>
       <c r="G261" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.2">
@@ -7635,7 +7638,7 @@
         <v>148</v>
       </c>
       <c r="G262" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.2">
@@ -7658,7 +7661,7 @@
         <v>148</v>
       </c>
       <c r="G263" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.2">
@@ -7681,7 +7684,7 @@
         <v>148</v>
       </c>
       <c r="G264" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.2">
@@ -7704,7 +7707,7 @@
         <v>148</v>
       </c>
       <c r="G265" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.2">
@@ -7727,7 +7730,7 @@
         <v>148</v>
       </c>
       <c r="G266" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.2">
@@ -7750,7 +7753,7 @@
         <v>148</v>
       </c>
       <c r="G267" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.2">
@@ -7773,7 +7776,7 @@
         <v>148</v>
       </c>
       <c r="G268" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.2">
@@ -7796,7 +7799,7 @@
         <v>148</v>
       </c>
       <c r="G269" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.2">
@@ -7819,7 +7822,7 @@
         <v>148</v>
       </c>
       <c r="G270" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.2">
@@ -7842,7 +7845,7 @@
         <v>148</v>
       </c>
       <c r="G271" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.2">
@@ -7865,7 +7868,7 @@
         <v>148</v>
       </c>
       <c r="G272" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.2">
@@ -7888,7 +7891,7 @@
         <v>148</v>
       </c>
       <c r="G273" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.2">
@@ -7911,7 +7914,7 @@
         <v>148</v>
       </c>
       <c r="G274" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.2">
@@ -7934,7 +7937,7 @@
         <v>148</v>
       </c>
       <c r="G275" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.2">
@@ -7957,7 +7960,7 @@
         <v>148</v>
       </c>
       <c r="G276" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.2">
@@ -7980,7 +7983,7 @@
         <v>148</v>
       </c>
       <c r="G277" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.2">
@@ -8003,7 +8006,7 @@
         <v>148</v>
       </c>
       <c r="G278" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.2">
@@ -8026,7 +8029,7 @@
         <v>148</v>
       </c>
       <c r="G279" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.2">
@@ -8049,7 +8052,7 @@
         <v>148</v>
       </c>
       <c r="G280" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.2">
@@ -8072,7 +8075,7 @@
         <v>148</v>
       </c>
       <c r="G281" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.2">
@@ -8095,7 +8098,7 @@
         <v>148</v>
       </c>
       <c r="G282" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.2">
@@ -8118,7 +8121,7 @@
         <v>148</v>
       </c>
       <c r="G283" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.2">
@@ -8141,7 +8144,7 @@
         <v>148</v>
       </c>
       <c r="G284" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added species id script for poc
</commit_message>
<xml_diff>
--- a/cites_list.xlsx
+++ b/cites_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E72609-CC0F-FD4C-850C-82E869CBAAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093D6272-6E0B-7043-85AF-1FC3F8D99CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="760" windowWidth="29240" windowHeight="17720" xr2:uid="{3910AC6C-398B-5641-A261-4AC5E77A0DDB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4691" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4696" uniqueCount="365">
   <si>
     <t>species</t>
   </si>
@@ -1122,6 +1122,15 @@
   </si>
   <si>
     <t>LEFT TO SHIP AS OF NOV 2024</t>
+  </si>
+  <si>
+    <t>To transport (all frozen)</t>
+  </si>
+  <si>
+    <t>ACR 2022 M1 box</t>
+  </si>
+  <si>
+    <t>ACR 2022 M2 box</t>
   </si>
 </sst>
 </file>
@@ -1193,13 +1202,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1514,11 +1524,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B8E095-94BA-A842-9ABD-01710D83669F}">
-  <dimension ref="A1:M577"/>
+  <dimension ref="A1:O577"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B532" sqref="B532"/>
+      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1532,7 +1542,7 @@
     <col min="15" max="15" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1561,7 +1571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>156</v>
       </c>
@@ -1595,7 +1605,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -1632,8 +1642,11 @@
       <c r="M3" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O3" s="6" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>156</v>
       </c>
@@ -1670,8 +1683,11 @@
       <c r="M4" s="3">
         <v>132</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>156</v>
       </c>
@@ -1706,8 +1722,11 @@
       <c r="M5" s="3">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>156</v>
       </c>
@@ -1742,8 +1761,11 @@
       <c r="M6" s="3">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>156</v>
       </c>
@@ -1778,8 +1800,11 @@
       <c r="M7" s="3">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O7" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>156</v>
       </c>
@@ -1811,7 +1836,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>156</v>
       </c>
@@ -1849,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>156</v>
       </c>
@@ -1885,7 +1910,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>156</v>
       </c>
@@ -1921,7 +1946,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>156</v>
       </c>
@@ -1953,7 +1978,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>156</v>
       </c>
@@ -1991,7 +2016,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>156</v>
       </c>
@@ -2027,7 +2052,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>156</v>
       </c>
@@ -2063,7 +2088,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>156</v>
       </c>

</xml_diff>